<commit_message>
Fixed clean_data_central_africa.xlsx bad index
* reset index before saving clean_data_central_africa.xlsx
</commit_message>
<xml_diff>
--- a/data/processed/clean_data_central_africa.xlsx
+++ b/data/processed/clean_data_central_africa.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="82">
   <si>
     <t>country_index</t>
   </si>
@@ -55,21 +55,21 @@
     <t>pct_agriculture_employment</t>
   </si>
   <si>
+    <t>pct_industry_employment</t>
+  </si>
+  <si>
+    <t>pct_services_employment</t>
+  </si>
+  <si>
+    <t>exports_pct_gdp</t>
+  </si>
+  <si>
+    <t>fdi_pct_gdp</t>
+  </si>
+  <si>
     <t>gni_index</t>
   </si>
   <si>
-    <t>pct_industry_employment</t>
-  </si>
-  <si>
-    <t>pct_services_employment</t>
-  </si>
-  <si>
-    <t>exports_pct_gdp</t>
-  </si>
-  <si>
-    <t>fdi_pct_gdp</t>
-  </si>
-  <si>
     <t>gdp_usd</t>
   </si>
   <si>
@@ -100,9 +100,6 @@
     <t>urban_population_growth_pct</t>
   </si>
   <si>
-    <t>m_income_group</t>
-  </si>
-  <si>
     <t>m_access_to_electricity_pop</t>
   </si>
   <si>
@@ -151,12 +148,6 @@
     <t>m_internet_usage_pct</t>
   </si>
   <si>
-    <t>m_homicides_per_100k</t>
-  </si>
-  <si>
-    <t>m_adult_literacy_pct</t>
-  </si>
-  <si>
     <t>m_child_mortality_per_1k</t>
   </si>
   <si>
@@ -164,9 +155,6 @@
   </si>
   <si>
     <t>m_women_in_parliament</t>
-  </si>
-  <si>
-    <t>m_tax_revenue_pct_gdp</t>
   </si>
   <si>
     <t>m_unemployment_pct</t>
@@ -629,13 +617,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BC15"/>
+  <dimension ref="A1:AY15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:55">
+    <row r="1" spans="1:51">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -786,37 +774,25 @@
       <c r="AY1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AZ1" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="BA1" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="BB1" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="BC1" s="1" t="s">
-        <v>53</v>
-      </c>
     </row>
-    <row r="2" spans="1:55">
+    <row r="2" spans="1:51">
       <c r="A2" s="1">
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="B2">
         <v>32</v>
       </c>
       <c r="C2" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D2" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E2" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="F2" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="G2">
         <v>7</v>
@@ -831,7 +807,7 @@
         <v>0.044485376</v>
       </c>
       <c r="K2">
-        <v>9.751295336787564</v>
+        <v>9.755208333333334</v>
       </c>
       <c r="L2">
         <v>12.70699978</v>
@@ -843,19 +819,19 @@
         <v>91.10299683</v>
       </c>
       <c r="O2">
+        <v>2.549000025</v>
+      </c>
+      <c r="P2">
+        <v>6.34800005</v>
+      </c>
+      <c r="Q2">
+        <v>7.76818252</v>
+      </c>
+      <c r="R2">
+        <v>2.642421428</v>
+      </c>
+      <c r="S2">
         <v>290</v>
-      </c>
-      <c r="P2">
-        <v>2.549000025</v>
-      </c>
-      <c r="Q2">
-        <v>6.34800005</v>
-      </c>
-      <c r="R2">
-        <v>7.76818252</v>
-      </c>
-      <c r="S2">
-        <v>2.642421428</v>
       </c>
       <c r="T2">
         <v>3093647227</v>
@@ -900,90 +876,78 @@
         <v>0</v>
       </c>
       <c r="AH2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI2">
+        <v>0</v>
+      </c>
+      <c r="AJ2">
+        <v>0</v>
+      </c>
+      <c r="AK2">
+        <v>0</v>
+      </c>
+      <c r="AL2">
+        <v>0</v>
+      </c>
+      <c r="AM2">
+        <v>0</v>
+      </c>
+      <c r="AN2">
+        <v>0</v>
+      </c>
+      <c r="AO2">
+        <v>0</v>
+      </c>
+      <c r="AP2">
+        <v>0</v>
+      </c>
+      <c r="AQ2">
+        <v>0</v>
+      </c>
+      <c r="AR2">
+        <v>0</v>
+      </c>
+      <c r="AS2">
+        <v>0</v>
+      </c>
+      <c r="AT2">
+        <v>0</v>
+      </c>
+      <c r="AU2">
+        <v>0</v>
+      </c>
+      <c r="AV2">
+        <v>0</v>
+      </c>
+      <c r="AW2">
+        <v>0</v>
+      </c>
+      <c r="AX2">
+        <v>0</v>
+      </c>
+      <c r="AY2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:51">
+      <c r="A3" s="1">
         <v>1</v>
-      </c>
-      <c r="AJ2">
-        <v>0</v>
-      </c>
-      <c r="AK2">
-        <v>0</v>
-      </c>
-      <c r="AL2">
-        <v>0</v>
-      </c>
-      <c r="AM2">
-        <v>0</v>
-      </c>
-      <c r="AN2">
-        <v>0</v>
-      </c>
-      <c r="AO2">
-        <v>0</v>
-      </c>
-      <c r="AP2">
-        <v>0</v>
-      </c>
-      <c r="AQ2">
-        <v>0</v>
-      </c>
-      <c r="AR2">
-        <v>0</v>
-      </c>
-      <c r="AS2">
-        <v>0</v>
-      </c>
-      <c r="AT2">
-        <v>0</v>
-      </c>
-      <c r="AU2">
-        <v>0</v>
-      </c>
-      <c r="AV2">
-        <v>0</v>
-      </c>
-      <c r="AW2">
-        <v>0</v>
-      </c>
-      <c r="AX2">
-        <v>0</v>
-      </c>
-      <c r="AY2">
-        <v>0</v>
-      </c>
-      <c r="AZ2">
-        <v>1</v>
-      </c>
-      <c r="BA2">
-        <v>0</v>
-      </c>
-      <c r="BB2">
-        <v>0</v>
-      </c>
-      <c r="BC2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:55">
-      <c r="A3" s="1">
-        <v>33</v>
       </c>
       <c r="B3">
         <v>33</v>
       </c>
       <c r="C3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D3" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="E3" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="F3" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="G3">
         <v>87.87672424</v>
@@ -1010,19 +974,19 @@
         <v>68.65499878</v>
       </c>
       <c r="O3">
+        <v>6.922999859</v>
+      </c>
+      <c r="P3">
+        <v>24.42200089</v>
+      </c>
+      <c r="Q3">
+        <v>40.36113967</v>
+      </c>
+      <c r="R3">
+        <v>9.718943229000001</v>
+      </c>
+      <c r="S3">
         <v>3310</v>
-      </c>
-      <c r="P3">
-        <v>6.922999859</v>
-      </c>
-      <c r="Q3">
-        <v>24.42200089</v>
-      </c>
-      <c r="R3">
-        <v>40.36113967</v>
-      </c>
-      <c r="S3">
-        <v>9.718943229000001</v>
       </c>
       <c r="T3">
         <v>1858121723</v>
@@ -1097,10 +1061,10 @@
         <v>0</v>
       </c>
       <c r="AR3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AS3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AT3">
         <v>0</v>
@@ -1109,7 +1073,7 @@
         <v>0</v>
       </c>
       <c r="AV3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AW3">
         <v>0</v>
@@ -1120,37 +1084,25 @@
       <c r="AY3">
         <v>0</v>
       </c>
-      <c r="AZ3">
-        <v>1</v>
-      </c>
-      <c r="BA3">
-        <v>0</v>
-      </c>
-      <c r="BB3">
-        <v>0</v>
-      </c>
-      <c r="BC3">
-        <v>0</v>
-      </c>
     </row>
-    <row r="4" spans="1:55">
+    <row r="4" spans="1:51">
       <c r="A4" s="1">
-        <v>44</v>
+        <v>2</v>
       </c>
       <c r="B4">
         <v>44</v>
       </c>
       <c r="C4" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D4" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="E4" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="F4" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="G4">
         <v>72.91772460999999</v>
@@ -1177,19 +1129,19 @@
         <v>54.98300171</v>
       </c>
       <c r="O4">
+        <v>15.57699966</v>
+      </c>
+      <c r="P4">
+        <v>29.44099998</v>
+      </c>
+      <c r="Q4">
+        <v>16.87471351</v>
+      </c>
+      <c r="R4">
+        <v>0.72227588</v>
+      </c>
+      <c r="S4">
         <v>830</v>
-      </c>
-      <c r="P4">
-        <v>15.57699966</v>
-      </c>
-      <c r="Q4">
-        <v>29.44099998</v>
-      </c>
-      <c r="R4">
-        <v>16.87471351</v>
-      </c>
-      <c r="S4">
-        <v>0.72227588</v>
       </c>
       <c r="T4">
         <v>647720707.1</v>
@@ -1273,10 +1225,10 @@
         <v>0</v>
       </c>
       <c r="AU4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AV4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AW4">
         <v>0</v>
@@ -1287,37 +1239,25 @@
       <c r="AY4">
         <v>0</v>
       </c>
-      <c r="AZ4">
-        <v>1</v>
-      </c>
-      <c r="BA4">
-        <v>0</v>
-      </c>
-      <c r="BB4">
-        <v>0</v>
-      </c>
-      <c r="BC4">
-        <v>0</v>
-      </c>
     </row>
-    <row r="5" spans="1:55">
+    <row r="5" spans="1:51">
       <c r="A5" s="1">
-        <v>45</v>
+        <v>3</v>
       </c>
       <c r="B5">
         <v>45</v>
       </c>
       <c r="C5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D5" t="s">
         <v>54</v>
       </c>
-      <c r="D5" t="s">
-        <v>58</v>
-      </c>
       <c r="E5" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="F5" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="G5">
         <v>13.5</v>
@@ -1344,19 +1284,19 @@
         <v>81.34899901999999</v>
       </c>
       <c r="O5">
+        <v>12.20400047</v>
+      </c>
+      <c r="P5">
+        <v>6.447000027</v>
+      </c>
+      <c r="Q5">
+        <v>36.83218885</v>
+      </c>
+      <c r="R5">
+        <v>5.131664248</v>
+      </c>
+      <c r="S5">
         <v>440</v>
-      </c>
-      <c r="P5">
-        <v>12.20400047</v>
-      </c>
-      <c r="Q5">
-        <v>6.447000027</v>
-      </c>
-      <c r="R5">
-        <v>36.83218885</v>
-      </c>
-      <c r="S5">
-        <v>5.131664248</v>
       </c>
       <c r="T5">
         <v>35917650630</v>
@@ -1440,10 +1380,10 @@
         <v>0</v>
       </c>
       <c r="AU5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AV5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AW5">
         <v>0</v>
@@ -1454,37 +1394,25 @@
       <c r="AY5">
         <v>0</v>
       </c>
-      <c r="AZ5">
-        <v>1</v>
-      </c>
-      <c r="BA5">
-        <v>0</v>
-      </c>
-      <c r="BB5">
-        <v>0</v>
-      </c>
-      <c r="BC5">
-        <v>0</v>
-      </c>
     </row>
-    <row r="6" spans="1:55">
+    <row r="6" spans="1:51">
       <c r="A6" s="1">
-        <v>46</v>
+        <v>4</v>
       </c>
       <c r="B6">
         <v>46</v>
       </c>
       <c r="C6" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D6" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="E6" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="F6" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="G6">
         <v>51.86239243</v>
@@ -1511,19 +1439,19 @@
         <v>38.22900009</v>
       </c>
       <c r="O6">
+        <v>25</v>
+      </c>
+      <c r="P6">
+        <v>36.77099991</v>
+      </c>
+      <c r="Q6">
+        <v>72.98675034</v>
+      </c>
+      <c r="R6">
+        <v>20.36515297</v>
+      </c>
+      <c r="S6">
         <v>2520</v>
-      </c>
-      <c r="P6">
-        <v>25</v>
-      </c>
-      <c r="Q6">
-        <v>36.77099991</v>
-      </c>
-      <c r="R6">
-        <v>72.98675034</v>
-      </c>
-      <c r="S6">
-        <v>20.36515297</v>
       </c>
       <c r="T6">
         <v>14177437982</v>
@@ -1607,10 +1535,10 @@
         <v>0</v>
       </c>
       <c r="AU6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AV6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AW6">
         <v>0</v>
@@ -1621,37 +1549,25 @@
       <c r="AY6">
         <v>0</v>
       </c>
-      <c r="AZ6">
-        <v>1</v>
-      </c>
-      <c r="BA6">
-        <v>0</v>
-      </c>
-      <c r="BB6">
-        <v>0</v>
-      </c>
-      <c r="BC6">
-        <v>0</v>
-      </c>
     </row>
-    <row r="7" spans="1:55">
+    <row r="7" spans="1:51">
       <c r="A7" s="1">
-        <v>48</v>
+        <v>5</v>
       </c>
       <c r="B7">
         <v>48</v>
       </c>
       <c r="C7" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D7" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="E7" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="F7" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="G7">
         <v>61.9</v>
@@ -1678,19 +1594,19 @@
         <v>50.375</v>
       </c>
       <c r="O7">
+        <v>5.986000061</v>
+      </c>
+      <c r="P7">
+        <v>43.63999939</v>
+      </c>
+      <c r="Q7">
+        <v>36.6588334</v>
+      </c>
+      <c r="R7">
+        <v>1.240430526</v>
+      </c>
+      <c r="S7">
         <v>1460</v>
-      </c>
-      <c r="P7">
-        <v>5.986000061</v>
-      </c>
-      <c r="Q7">
-        <v>43.63999939</v>
-      </c>
-      <c r="R7">
-        <v>36.6588334</v>
-      </c>
-      <c r="S7">
-        <v>1.240430526</v>
       </c>
       <c r="T7">
         <v>35372603446</v>
@@ -1774,7 +1690,7 @@
         <v>0</v>
       </c>
       <c r="AU7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AV7">
         <v>0</v>
@@ -1788,37 +1704,25 @@
       <c r="AY7">
         <v>0</v>
       </c>
-      <c r="AZ7">
-        <v>0</v>
-      </c>
-      <c r="BA7">
-        <v>0</v>
-      </c>
-      <c r="BB7">
-        <v>0</v>
-      </c>
-      <c r="BC7">
-        <v>0</v>
-      </c>
     </row>
-    <row r="8" spans="1:55">
+    <row r="8" spans="1:51">
       <c r="A8" s="1">
-        <v>61</v>
+        <v>6</v>
       </c>
       <c r="B8">
         <v>61</v>
       </c>
       <c r="C8" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D8" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E8" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="F8" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="G8">
         <v>67.05870819</v>
@@ -1845,19 +1749,19 @@
         <v>54.96300125</v>
       </c>
       <c r="O8">
+        <v>8.237000464999999</v>
+      </c>
+      <c r="P8">
+        <v>36.79999924</v>
+      </c>
+      <c r="Q8">
+        <v>65.9632886</v>
+      </c>
+      <c r="R8">
+        <v>0.772319187</v>
+      </c>
+      <c r="S8">
         <v>13140</v>
-      </c>
-      <c r="P8">
-        <v>8.237000464999999</v>
-      </c>
-      <c r="Q8">
-        <v>36.79999924</v>
-      </c>
-      <c r="R8">
-        <v>65.9632886</v>
-      </c>
-      <c r="S8">
-        <v>0.772319187</v>
       </c>
       <c r="T8">
         <v>21736500713</v>
@@ -1941,10 +1845,10 @@
         <v>0</v>
       </c>
       <c r="AU8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AV8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AW8">
         <v>0</v>
@@ -1955,37 +1859,25 @@
       <c r="AY8">
         <v>0</v>
       </c>
-      <c r="AZ8">
-        <v>0</v>
-      </c>
-      <c r="BA8">
-        <v>0</v>
-      </c>
-      <c r="BB8">
-        <v>0</v>
-      </c>
-      <c r="BC8">
-        <v>0</v>
-      </c>
     </row>
-    <row r="9" spans="1:55">
+    <row r="9" spans="1:51">
       <c r="A9" s="1">
-        <v>75</v>
+        <v>7</v>
       </c>
       <c r="B9">
         <v>74</v>
       </c>
       <c r="C9" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D9" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E9" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F9" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="G9">
         <v>78.3</v>
@@ -2012,19 +1904,19 @@
         <v>44.72000122</v>
       </c>
       <c r="O9">
+        <v>14.10700035</v>
+      </c>
+      <c r="P9">
+        <v>41.17300034</v>
+      </c>
+      <c r="Q9">
+        <v>39.52355867</v>
+      </c>
+      <c r="R9">
+        <v>8.604962551</v>
+      </c>
+      <c r="S9">
         <v>1590</v>
-      </c>
-      <c r="P9">
-        <v>14.10700035</v>
-      </c>
-      <c r="Q9">
-        <v>41.17300034</v>
-      </c>
-      <c r="R9">
-        <v>39.52355867</v>
-      </c>
-      <c r="S9">
-        <v>8.604962551</v>
       </c>
       <c r="T9">
         <v>39086625009</v>
@@ -2108,10 +2000,10 @@
         <v>0</v>
       </c>
       <c r="AU9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AV9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AW9">
         <v>0</v>
@@ -2122,37 +2014,25 @@
       <c r="AY9">
         <v>0</v>
       </c>
-      <c r="AZ9">
-        <v>1</v>
-      </c>
-      <c r="BA9">
-        <v>0</v>
-      </c>
-      <c r="BB9">
-        <v>0</v>
-      </c>
-      <c r="BC9">
-        <v>0</v>
-      </c>
     </row>
-    <row r="10" spans="1:55">
+    <row r="10" spans="1:51">
       <c r="A10" s="1">
-        <v>102</v>
+        <v>8</v>
       </c>
       <c r="B10">
         <v>101</v>
       </c>
       <c r="C10" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D10" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E10" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="F10" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="G10">
         <v>36</v>
@@ -2179,19 +2059,19 @@
         <v>37.63899994</v>
       </c>
       <c r="O10">
+        <v>14.90200043</v>
+      </c>
+      <c r="P10">
+        <v>47.45899963</v>
+      </c>
+      <c r="Q10">
+        <v>18.29698092</v>
+      </c>
+      <c r="R10">
+        <v>1.335986481</v>
+      </c>
+      <c r="S10">
         <v>1260</v>
-      </c>
-      <c r="P10">
-        <v>14.90200043</v>
-      </c>
-      <c r="Q10">
-        <v>47.45899963</v>
-      </c>
-      <c r="R10">
-        <v>18.29698092</v>
-      </c>
-      <c r="S10">
-        <v>1.335986481</v>
       </c>
       <c r="T10">
         <v>61448046802</v>
@@ -2289,37 +2169,25 @@
       <c r="AY10">
         <v>0</v>
       </c>
-      <c r="AZ10">
-        <v>0</v>
-      </c>
-      <c r="BA10">
-        <v>0</v>
-      </c>
-      <c r="BB10">
-        <v>0</v>
-      </c>
-      <c r="BC10">
-        <v>0</v>
-      </c>
     </row>
-    <row r="11" spans="1:55">
+    <row r="11" spans="1:51">
       <c r="A11" s="1">
-        <v>146</v>
+        <v>9</v>
       </c>
       <c r="B11">
         <v>145</v>
       </c>
       <c r="C11" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D11" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="E11" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="F11" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="G11">
         <v>56.37191391</v>
@@ -2346,19 +2214,19 @@
         <v>36.77999878</v>
       </c>
       <c r="O11">
+        <v>12.06200027</v>
+      </c>
+      <c r="P11">
+        <v>51.1590004</v>
+      </c>
+      <c r="Q11">
+        <v>18.43512605</v>
+      </c>
+      <c r="R11">
+        <v>0.818201344</v>
+      </c>
+      <c r="S11">
         <v>2980</v>
-      </c>
-      <c r="P11">
-        <v>12.06200027</v>
-      </c>
-      <c r="Q11">
-        <v>51.1590004</v>
-      </c>
-      <c r="R11">
-        <v>18.43512605</v>
-      </c>
-      <c r="S11">
-        <v>0.818201344</v>
       </c>
       <c r="T11">
         <v>568499000000</v>
@@ -2442,10 +2310,10 @@
         <v>0</v>
       </c>
       <c r="AU11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AV11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AW11">
         <v>0</v>
@@ -2456,37 +2324,25 @@
       <c r="AY11">
         <v>0</v>
       </c>
-      <c r="AZ11">
-        <v>1</v>
-      </c>
-      <c r="BA11">
-        <v>0</v>
-      </c>
-      <c r="BB11">
-        <v>0</v>
-      </c>
-      <c r="BC11">
-        <v>0</v>
-      </c>
     </row>
-    <row r="12" spans="1:55">
+    <row r="12" spans="1:51">
       <c r="A12" s="1">
-        <v>163</v>
+        <v>10</v>
       </c>
       <c r="B12">
         <v>162</v>
       </c>
       <c r="C12" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D12" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E12" t="s">
+        <v>75</v>
+      </c>
+      <c r="F12" t="s">
         <v>79</v>
-      </c>
-      <c r="F12" t="s">
-        <v>83</v>
       </c>
       <c r="G12">
         <v>19.8</v>
@@ -2513,19 +2369,19 @@
         <v>68.45300293</v>
       </c>
       <c r="O12">
+        <v>7.913000107</v>
+      </c>
+      <c r="P12">
+        <v>23.63400078</v>
+      </c>
+      <c r="Q12">
+        <v>14.72211453</v>
+      </c>
+      <c r="R12">
+        <v>3.926137464</v>
+      </c>
+      <c r="S12">
         <v>700</v>
-      </c>
-      <c r="P12">
-        <v>7.913000107</v>
-      </c>
-      <c r="Q12">
-        <v>23.63400078</v>
-      </c>
-      <c r="R12">
-        <v>14.72211453</v>
-      </c>
-      <c r="S12">
-        <v>3.926137464</v>
       </c>
       <c r="T12">
         <v>8016591928</v>
@@ -2609,10 +2465,10 @@
         <v>0</v>
       </c>
       <c r="AU12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AV12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AW12">
         <v>0</v>
@@ -2623,37 +2479,25 @@
       <c r="AY12">
         <v>0</v>
       </c>
-      <c r="AZ12">
-        <v>0</v>
-      </c>
-      <c r="BA12">
-        <v>0</v>
-      </c>
-      <c r="BB12">
-        <v>0</v>
-      </c>
-      <c r="BC12">
-        <v>0</v>
-      </c>
     </row>
-    <row r="13" spans="1:55">
+    <row r="13" spans="1:51">
       <c r="A13" s="1">
-        <v>168</v>
+        <v>11</v>
       </c>
       <c r="B13">
         <v>167</v>
       </c>
       <c r="C13" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D13" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E13" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="F13" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="G13">
         <v>61</v>
@@ -2680,19 +2524,19 @@
         <v>53.67399979</v>
       </c>
       <c r="O13">
+        <v>20.20499992</v>
+      </c>
+      <c r="P13">
+        <v>26.12100029</v>
+      </c>
+      <c r="Q13">
+        <v>28.12071229</v>
+      </c>
+      <c r="R13">
+        <v>2.630373382</v>
+      </c>
+      <c r="S13">
         <v>1030</v>
-      </c>
-      <c r="P13">
-        <v>20.20499992</v>
-      </c>
-      <c r="Q13">
-        <v>26.12100029</v>
-      </c>
-      <c r="R13">
-        <v>28.12071229</v>
-      </c>
-      <c r="S13">
-        <v>2.630373382</v>
       </c>
       <c r="T13">
         <v>15304363138</v>
@@ -2776,10 +2620,10 @@
         <v>0</v>
       </c>
       <c r="AU13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AV13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AW13">
         <v>0</v>
@@ -2790,37 +2634,25 @@
       <c r="AY13">
         <v>0</v>
       </c>
-      <c r="AZ13">
-        <v>0</v>
-      </c>
-      <c r="BA13">
-        <v>0</v>
-      </c>
-      <c r="BB13">
-        <v>0</v>
-      </c>
-      <c r="BC13">
-        <v>0</v>
-      </c>
     </row>
-    <row r="14" spans="1:55">
+    <row r="14" spans="1:51">
       <c r="A14" s="1">
-        <v>186</v>
+        <v>12</v>
       </c>
       <c r="B14">
         <v>185</v>
       </c>
       <c r="C14" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D14" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="E14" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="F14" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="G14">
         <v>44.9</v>
@@ -2847,19 +2679,19 @@
         <v>53.35599899</v>
       </c>
       <c r="O14">
+        <v>18.83399963</v>
+      </c>
+      <c r="P14">
+        <v>27.80999947</v>
+      </c>
+      <c r="Q14">
+        <v>8.149134518</v>
+      </c>
+      <c r="R14">
+        <v>1.523136574</v>
+      </c>
+      <c r="S14">
         <v>1830</v>
-      </c>
-      <c r="P14">
-        <v>18.83399963</v>
-      </c>
-      <c r="Q14">
-        <v>27.80999947</v>
-      </c>
-      <c r="R14">
-        <v>8.149134518</v>
-      </c>
-      <c r="S14">
-        <v>1.523136574</v>
       </c>
       <c r="T14">
         <v>82151588419</v>
@@ -2943,10 +2775,10 @@
         <v>0</v>
       </c>
       <c r="AU14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AV14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AW14">
         <v>0</v>
@@ -2957,37 +2789,25 @@
       <c r="AY14">
         <v>0</v>
       </c>
-      <c r="AZ14">
-        <v>1</v>
-      </c>
-      <c r="BA14">
-        <v>0</v>
-      </c>
-      <c r="BB14">
-        <v>0</v>
-      </c>
-      <c r="BC14">
-        <v>0</v>
-      </c>
     </row>
-    <row r="15" spans="1:55">
+    <row r="15" spans="1:51">
       <c r="A15" s="1">
-        <v>203</v>
+        <v>13</v>
       </c>
       <c r="B15">
         <v>203</v>
       </c>
       <c r="C15" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D15" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="E15" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="F15" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="G15">
         <v>20.4</v>
@@ -3014,19 +2834,19 @@
         <v>71.54699707</v>
       </c>
       <c r="O15">
+        <v>6.887000084</v>
+      </c>
+      <c r="P15">
+        <v>21.56500053</v>
+      </c>
+      <c r="Q15">
+        <v>18.17025675</v>
+      </c>
+      <c r="R15">
+        <v>3.878679401</v>
+      </c>
+      <c r="S15">
         <v>660</v>
-      </c>
-      <c r="P15">
-        <v>6.887000084</v>
-      </c>
-      <c r="Q15">
-        <v>21.56500053</v>
-      </c>
-      <c r="R15">
-        <v>18.17025675</v>
-      </c>
-      <c r="S15">
-        <v>3.878679401</v>
       </c>
       <c r="T15">
         <v>27291880327</v>
@@ -3113,7 +2933,7 @@
         <v>0</v>
       </c>
       <c r="AV15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AW15">
         <v>0</v>
@@ -3122,18 +2942,6 @@
         <v>0</v>
       </c>
       <c r="AY15">
-        <v>0</v>
-      </c>
-      <c r="AZ15">
-        <v>1</v>
-      </c>
-      <c r="BA15">
-        <v>0</v>
-      </c>
-      <c r="BB15">
-        <v>0</v>
-      </c>
-      <c r="BC15">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
v1.0.0 use __main__.py to run the project
</commit_message>
<xml_diff>
--- a/data/processed/clean_data_central_africa.xlsx
+++ b/data/processed/clean_data_central_africa.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="85">
   <si>
     <t>country_index</t>
   </si>
@@ -164,6 +164,15 @@
   </si>
   <si>
     <t>m_urban_population_growth_pct</t>
+  </si>
+  <si>
+    <t>m_adult_literacy_pct</t>
+  </si>
+  <si>
+    <t>m_homicides_per_100k</t>
+  </si>
+  <si>
+    <t>m_tax_revenue_pct_gdp</t>
   </si>
   <si>
     <t>Central Africa 1</t>
@@ -617,13 +626,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AY15"/>
+  <dimension ref="A1:BB15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:51">
+    <row r="1" spans="1:54">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -774,8 +783,17 @@
       <c r="AY1" s="1" t="s">
         <v>49</v>
       </c>
+      <c r="AZ1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="BA1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="BB1" s="1" t="s">
+        <v>52</v>
+      </c>
     </row>
-    <row r="2" spans="1:51">
+    <row r="2" spans="1:54">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -783,16 +801,16 @@
         <v>32</v>
       </c>
       <c r="C2" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="D2" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="E2" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="F2" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="G2">
         <v>7</v>
@@ -929,8 +947,17 @@
       <c r="AY2">
         <v>0</v>
       </c>
+      <c r="AZ2">
+        <v>0</v>
+      </c>
+      <c r="BA2">
+        <v>0</v>
+      </c>
+      <c r="BB2">
+        <v>1</v>
+      </c>
     </row>
-    <row r="3" spans="1:51">
+    <row r="3" spans="1:54">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -938,16 +965,16 @@
         <v>44</v>
       </c>
       <c r="C3" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="D3" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="E3" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="F3" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="G3">
         <v>72.91772460999999</v>
@@ -1084,8 +1111,17 @@
       <c r="AY3">
         <v>0</v>
       </c>
+      <c r="AZ3">
+        <v>1</v>
+      </c>
+      <c r="BA3">
+        <v>1</v>
+      </c>
+      <c r="BB3">
+        <v>1</v>
+      </c>
     </row>
-    <row r="4" spans="1:51">
+    <row r="4" spans="1:54">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1093,16 +1129,16 @@
         <v>46</v>
       </c>
       <c r="C4" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="D4" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="E4" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="F4" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="G4">
         <v>51.86239243</v>
@@ -1239,8 +1275,17 @@
       <c r="AY4">
         <v>0</v>
       </c>
+      <c r="AZ4">
+        <v>1</v>
+      </c>
+      <c r="BA4">
+        <v>1</v>
+      </c>
+      <c r="BB4">
+        <v>1</v>
+      </c>
     </row>
-    <row r="5" spans="1:51">
+    <row r="5" spans="1:54">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1248,16 +1293,16 @@
         <v>162</v>
       </c>
       <c r="C5" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="D5" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="E5" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="F5" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="G5">
         <v>19.8</v>
@@ -1394,8 +1439,17 @@
       <c r="AY5">
         <v>0</v>
       </c>
+      <c r="AZ5">
+        <v>1</v>
+      </c>
+      <c r="BA5">
+        <v>1</v>
+      </c>
+      <c r="BB5">
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:51">
+    <row r="6" spans="1:54">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1403,16 +1457,16 @@
         <v>167</v>
       </c>
       <c r="C6" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="D6" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="E6" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="F6" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="G6">
         <v>61</v>
@@ -1549,8 +1603,17 @@
       <c r="AY6">
         <v>0</v>
       </c>
+      <c r="AZ6">
+        <v>1</v>
+      </c>
+      <c r="BA6">
+        <v>1</v>
+      </c>
+      <c r="BB6">
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" spans="1:51">
+    <row r="7" spans="1:54">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1558,16 +1621,16 @@
         <v>203</v>
       </c>
       <c r="C7" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="D7" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="E7" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="F7" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="G7">
         <v>20.4</v>
@@ -1704,8 +1767,17 @@
       <c r="AY7">
         <v>0</v>
       </c>
+      <c r="AZ7">
+        <v>1</v>
+      </c>
+      <c r="BA7">
+        <v>0</v>
+      </c>
+      <c r="BB7">
+        <v>1</v>
+      </c>
     </row>
-    <row r="8" spans="1:51">
+    <row r="8" spans="1:54">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1713,16 +1785,16 @@
         <v>61</v>
       </c>
       <c r="C8" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="D8" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="E8" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="F8" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="G8">
         <v>67.05870819</v>
@@ -1859,8 +1931,17 @@
       <c r="AY8">
         <v>0</v>
       </c>
+      <c r="AZ8">
+        <v>1</v>
+      </c>
+      <c r="BA8">
+        <v>1</v>
+      </c>
+      <c r="BB8">
+        <v>0</v>
+      </c>
     </row>
-    <row r="9" spans="1:51">
+    <row r="9" spans="1:54">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1868,16 +1949,16 @@
         <v>33</v>
       </c>
       <c r="C9" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="D9" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="E9" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="F9" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="G9">
         <v>87.87672424</v>
@@ -2014,8 +2095,17 @@
       <c r="AY9">
         <v>0</v>
       </c>
+      <c r="AZ9">
+        <v>1</v>
+      </c>
+      <c r="BA9">
+        <v>0</v>
+      </c>
+      <c r="BB9">
+        <v>1</v>
+      </c>
     </row>
-    <row r="10" spans="1:51">
+    <row r="10" spans="1:54">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -2023,16 +2113,16 @@
         <v>45</v>
       </c>
       <c r="C10" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="D10" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="E10" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="F10" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="G10">
         <v>13.5</v>
@@ -2169,8 +2259,17 @@
       <c r="AY10">
         <v>0</v>
       </c>
+      <c r="AZ10">
+        <v>1</v>
+      </c>
+      <c r="BA10">
+        <v>1</v>
+      </c>
+      <c r="BB10">
+        <v>1</v>
+      </c>
     </row>
-    <row r="11" spans="1:51">
+    <row r="11" spans="1:54">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -2178,16 +2277,16 @@
         <v>48</v>
       </c>
       <c r="C11" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="D11" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="E11" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="F11" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="G11">
         <v>61.9</v>
@@ -2324,8 +2423,17 @@
       <c r="AY11">
         <v>0</v>
       </c>
+      <c r="AZ11">
+        <v>0</v>
+      </c>
+      <c r="BA11">
+        <v>1</v>
+      </c>
+      <c r="BB11">
+        <v>0</v>
+      </c>
     </row>
-    <row r="12" spans="1:51">
+    <row r="12" spans="1:54">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -2333,16 +2441,16 @@
         <v>74</v>
       </c>
       <c r="C12" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="D12" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="E12" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="F12" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="G12">
         <v>78.3</v>
@@ -2479,8 +2587,17 @@
       <c r="AY12">
         <v>0</v>
       </c>
+      <c r="AZ12">
+        <v>1</v>
+      </c>
+      <c r="BA12">
+        <v>1</v>
+      </c>
+      <c r="BB12">
+        <v>1</v>
+      </c>
     </row>
-    <row r="13" spans="1:51">
+    <row r="13" spans="1:54">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -2488,16 +2605,16 @@
         <v>101</v>
       </c>
       <c r="C13" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="D13" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="E13" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="F13" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="G13">
         <v>36</v>
@@ -2634,8 +2751,17 @@
       <c r="AY13">
         <v>0</v>
       </c>
+      <c r="AZ13">
+        <v>0</v>
+      </c>
+      <c r="BA13">
+        <v>0</v>
+      </c>
+      <c r="BB13">
+        <v>0</v>
+      </c>
     </row>
-    <row r="14" spans="1:51">
+    <row r="14" spans="1:54">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -2643,16 +2769,16 @@
         <v>145</v>
       </c>
       <c r="C14" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="D14" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="E14" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="F14" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="G14">
         <v>56.37191391</v>
@@ -2789,8 +2915,17 @@
       <c r="AY14">
         <v>0</v>
       </c>
+      <c r="AZ14">
+        <v>1</v>
+      </c>
+      <c r="BA14">
+        <v>1</v>
+      </c>
+      <c r="BB14">
+        <v>1</v>
+      </c>
     </row>
-    <row r="15" spans="1:51">
+    <row r="15" spans="1:54">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -2798,16 +2933,16 @@
         <v>185</v>
       </c>
       <c r="C15" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="D15" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="E15" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="F15" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="G15">
         <v>44.9</v>
@@ -2943,6 +3078,15 @@
       </c>
       <c r="AY15">
         <v>0</v>
+      </c>
+      <c r="AZ15">
+        <v>1</v>
+      </c>
+      <c r="BA15">
+        <v>1</v>
+      </c>
+      <c r="BB15">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>